<commit_message>
Final data + Report.
</commit_message>
<xml_diff>
--- a/matrixmult-openmp/OpenMP-Speeds-Kali-Linux.xlsx
+++ b/matrixmult-openmp/OpenMP-Speeds-Kali-Linux.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fsociety/Desktop/Senior Year/Spring 2023/CSC447 - Parallel Progg:Multic.&amp;Cluster/SharedMem/matrixmult-openmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75554D90-C640-F841-9F76-09FC7CE33410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C48B60-4493-3B43-BA5B-DB9E7B1A3F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{9AC2A181-F548-9547-B226-FB9881CBD48A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$78</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Matrix Size</t>
   </si>
@@ -46,22 +50,21 @@
   <si>
     <t>Number of Threads</t>
   </si>
+  <si>
+    <t>Speed Up</t>
+  </si>
+  <si>
+    <t>Effeciency</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,9 +90,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -286,10 +288,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$9:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>500</c:v>
                 </c:pt>
@@ -311,41 +313,35 @@
                 <c:pt idx="6">
                   <c:v>3500</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>4000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$9:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0224500000000001</c:v>
+                  <c:v>1.0037069999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0497290000000001</c:v>
+                  <c:v>2.0201850000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4193100000000003</c:v>
+                  <c:v>6.4811170000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.821032000000001</c:v>
+                  <c:v>15.742611999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.054715999999999</c:v>
+                  <c:v>32.072834</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.125656000000006</c:v>
+                  <c:v>73.658243999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>309.07380599999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>453.45042000000001</c:v>
+                  <c:v>231.30529899999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,7 +1101,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>314960</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1431,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F9117C-B124-2445-811A-AF9A52053590}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1457,79 +1453,79 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
       <c r="C2">
-        <v>1.0224500000000001</v>
+        <v>1.0083930000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>2.0497290000000001</v>
+        <v>3.6775720000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>1500</v>
       </c>
       <c r="C4">
-        <v>6.4193100000000003</v>
+        <v>13.284219</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5">
-        <v>15.821032000000001</v>
+        <v>32.286002000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>2500</v>
       </c>
       <c r="C6">
-        <v>32.054715999999999</v>
+        <v>58.90352</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>3000</v>
       </c>
       <c r="C7">
-        <v>74.125656000000006</v>
+        <v>115.60058100000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>3500</v>
       </c>
       <c r="C8">
-        <v>309.07380599999999</v>
+        <v>324.50760500000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1537,630 +1533,1020 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="C9">
-        <v>453.45042000000001</v>
+        <v>1.0037069999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C10">
-        <v>0.60992599999999997</v>
+        <v>2.0201850000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="C11">
-        <v>1.616174</v>
+        <v>6.4811170000000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="C12">
-        <v>3.9298289999999998</v>
+        <v>15.742611999999999</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="C13">
-        <v>8.8307359999999999</v>
+        <v>32.072834</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="C14">
-        <v>17.431992999999999</v>
+        <v>73.658243999999996</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="C15">
-        <v>65.381985</v>
+        <v>231.30529899999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="C16">
-        <v>328.521503</v>
+        <v>0.48128799999999999</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="C17">
-        <v>526.01597600000002</v>
+        <v>1.7833289999999999</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="C18">
-        <v>0.12948299999999999</v>
+        <v>5.1064189999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C19">
-        <v>1.0398069999999999</v>
+        <v>10.580284000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="C20">
-        <v>3.1728580000000002</v>
+        <v>21.222936000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="C21">
-        <v>7.6619460000000004</v>
+        <v>63.231437</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C22">
-        <v>15.752941</v>
+        <v>331.25501100000002</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="C23">
-        <v>54.885849999999998</v>
+        <v>0.39424199999999998</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24">
-        <v>3500</v>
+        <v>1000</v>
       </c>
       <c r="C24">
-        <v>214.95491999999999</v>
+        <v>1.3802350000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="C25">
-        <v>262.38910299999998</v>
+        <v>3.6715230000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="C26">
-        <v>0.493757</v>
+        <v>8.5206350000000004</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C27">
-        <v>1.398455</v>
+        <v>16.243614999999998</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="C28">
-        <v>3.6087509999999998</v>
+        <v>59.197105000000001</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>2000</v>
+        <v>3500</v>
       </c>
       <c r="C29">
-        <v>8.2871120000000005</v>
+        <v>335.76788299999998</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="C30">
-        <v>15.206858</v>
+        <v>0.90999200000000002</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="C31">
-        <v>51.852901000000003</v>
+        <v>1.8591500000000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>3500</v>
+        <v>1500</v>
       </c>
       <c r="C32">
-        <v>210.695212</v>
+        <v>4.0840430000000003</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B33">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="C33">
-        <v>322.30694</v>
+        <v>7.7449170000000001</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B34">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="C34">
-        <v>0.42121700000000001</v>
+        <v>16.035886999999999</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C35">
-        <v>1.324363</v>
+        <v>53.995655999999997</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B36">
-        <v>1500</v>
+        <v>3500</v>
       </c>
       <c r="C36">
-        <v>3.505363</v>
+        <v>247.789243</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B37">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C37">
-        <v>8.1188020000000005</v>
+        <v>0.91275200000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B38">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="C38">
-        <v>14.979492</v>
+        <v>1.819968</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B39">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="C39">
-        <v>52.096707000000002</v>
+        <v>3.9356260000000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B40">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="C40">
-        <v>209.76459</v>
+        <v>8.4012259999999994</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B41">
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="C41">
-        <v>335.56713500000001</v>
+        <v>15.264246</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B42">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="C42">
-        <v>0.69291000000000003</v>
+        <v>51.569125</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B43">
-        <v>1000</v>
+        <v>3500</v>
       </c>
       <c r="C43">
-        <v>1.5999140000000001</v>
+        <v>197.23310900000001</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B44">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="C44">
-        <v>3.7848670000000002</v>
+        <v>0.35199200000000003</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B45">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="C45">
-        <v>8.6588049999999992</v>
+        <v>1.257884</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B46">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="C46">
-        <v>15.806896999999999</v>
+        <v>3.375092</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B47">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C47">
-        <v>52.542470999999999</v>
+        <v>7.9933059999999996</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B48">
-        <v>3500</v>
+        <v>2500</v>
       </c>
       <c r="C48">
-        <v>209.93044699999999</v>
+        <v>15.012578</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B49">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C49">
-        <v>324.55775399999999</v>
+        <v>51.721136999999999</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B50">
-        <v>500</v>
+        <v>3500</v>
       </c>
       <c r="C50">
-        <v>0.69</v>
+        <v>206.013724</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B51">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C51">
-        <v>1.6521049999999999</v>
+        <v>0.13156899999999999</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B52">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="C52">
-        <v>3.9667050000000001</v>
+        <v>1.0337769999999999</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B53">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="C53">
-        <v>8.5995399999999993</v>
+        <v>3.1978240000000002</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B54">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="C54">
-        <v>15.951264</v>
+        <v>8.7107949999999992</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B55">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="C55">
-        <v>54.391210000000001</v>
+        <v>16.422861999999999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B56">
-        <v>3500</v>
+        <v>3000</v>
       </c>
       <c r="C56">
-        <v>213.286168</v>
+        <v>51.646286000000003</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B57">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="C57">
-        <v>327.37002699999999</v>
+        <v>207.410155</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>16</v>
-      </c>
-      <c r="B58" s="1">
+        <v>9</v>
+      </c>
+      <c r="B58">
         <v>500</v>
       </c>
       <c r="C58">
-        <v>0.497614</v>
+        <v>0.53719099999999997</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>16</v>
-      </c>
-      <c r="B59" s="1">
+        <v>9</v>
+      </c>
+      <c r="B59">
         <v>1000</v>
       </c>
       <c r="C59">
-        <v>1.3983760000000001</v>
+        <v>1.4999610000000001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>16</v>
-      </c>
-      <c r="B60" s="1">
+        <v>9</v>
+      </c>
+      <c r="B60">
         <v>1500</v>
       </c>
       <c r="C60">
-        <v>3.6112959999999998</v>
+        <v>3.6425969999999999</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>16</v>
-      </c>
-      <c r="B61" s="1">
+        <v>9</v>
+      </c>
+      <c r="B61">
         <v>2000</v>
       </c>
       <c r="C61">
-        <v>8.2469560000000008</v>
+        <v>7.9931799999999997</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>16</v>
-      </c>
-      <c r="B62" s="1">
+        <v>9</v>
+      </c>
+      <c r="B62">
         <v>2500</v>
       </c>
       <c r="C62">
-        <v>14.995200000000001</v>
+        <v>14.957231999999999</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>16</v>
-      </c>
-      <c r="B63" s="1">
+        <v>9</v>
+      </c>
+      <c r="B63">
         <v>3000</v>
       </c>
       <c r="C63">
-        <v>49.770457</v>
+        <v>50.857154999999999</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>16</v>
-      </c>
-      <c r="B64" s="1">
+        <v>9</v>
+      </c>
+      <c r="B64">
         <v>3500</v>
       </c>
       <c r="C64">
-        <v>211.510054</v>
+        <v>209.51456200000001</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>16</v>
-      </c>
-      <c r="B65" s="1">
-        <v>4000</v>
+        <v>10</v>
+      </c>
+      <c r="B65">
+        <v>500</v>
       </c>
       <c r="C65">
-        <v>325.83576599999998</v>
+        <v>0.46051199999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>1000</v>
+      </c>
+      <c r="C66">
+        <v>1.3933530000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>1500</v>
+      </c>
+      <c r="C67">
+        <v>3.5963370000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>2000</v>
+      </c>
+      <c r="C68">
+        <v>8.0948689999999992</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>2500</v>
+      </c>
+      <c r="C69">
+        <v>15.160802</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70">
+        <v>3000</v>
+      </c>
+      <c r="C70">
+        <v>51.536740999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>3500</v>
+      </c>
+      <c r="C71">
+        <v>208.838863</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="B72">
+        <v>500</v>
+      </c>
+      <c r="C72">
+        <v>0.96038999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>11</v>
+      </c>
+      <c r="B73">
+        <v>1000</v>
+      </c>
+      <c r="C73">
+        <v>1.8790420000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>11</v>
+      </c>
+      <c r="B74">
+        <v>1500</v>
+      </c>
+      <c r="C74">
+        <v>4.0056279999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>11</v>
+      </c>
+      <c r="B75">
+        <v>2000</v>
+      </c>
+      <c r="C75">
+        <v>7.6029070000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <v>2500</v>
+      </c>
+      <c r="C76">
+        <v>15.468503</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>11</v>
+      </c>
+      <c r="B77">
+        <v>3000</v>
+      </c>
+      <c r="C77">
+        <v>51.316721000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>11</v>
+      </c>
+      <c r="B78">
+        <v>3500</v>
+      </c>
+      <c r="C78">
+        <v>212.680825</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B78" xr:uid="{92F9117C-B124-2445-811A-AF9A52053590}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82614BF9-4F40-A547-A741-7775124BDCC8}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3000</v>
+      </c>
+      <c r="C2">
+        <v>115.60058100000001</v>
+      </c>
+      <c r="D2">
+        <f>C2/C2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>D2/A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3000</v>
+      </c>
+      <c r="C3">
+        <v>73.658243999999996</v>
+      </c>
+      <c r="D3">
+        <f>$C$2/C3</f>
+        <v>1.5694180952779706</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E12" si="0">D3/A3</f>
+        <v>0.7847090476389853</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4">
+        <v>63.231437</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D12" si="1">$C$2/C4</f>
+        <v>1.8282137253973842</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.60940457513246138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3000</v>
+      </c>
+      <c r="C5">
+        <v>59.197105000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1.9528080131621302</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.48820200329053254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3000</v>
+      </c>
+      <c r="C6">
+        <v>53.995655999999997</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.1409237254196896</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.42818474508393789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3000</v>
+      </c>
+      <c r="C7">
+        <v>51.569125</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2.2416626421332535</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.37361044035554225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3000</v>
+      </c>
+      <c r="C8">
+        <v>51.721136999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>2.2350742405372874</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.31929632007675535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3000</v>
+      </c>
+      <c r="C9">
+        <v>51.646286000000003</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.2383135352656334</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.27978919190820417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3000</v>
+      </c>
+      <c r="C10">
+        <v>50.857154999999999</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>2.2730445893011515</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.25256050992235018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3000</v>
+      </c>
+      <c r="C11">
+        <v>51.536740999999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.2430712295137174</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.22430712295137173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3000</v>
+      </c>
+      <c r="C12">
+        <v>51.316721000000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2.2526883781214315</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.20478985255649376</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>